<commit_message>
eliminada lib descargada, trabajando todo con pom.xml
</commit_message>
<xml_diff>
--- a/src/ficheros/inf1.xlsx
+++ b/src/ficheros/inf1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Código</t>
   </si>
@@ -38,13 +38,13 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Pepe</t>
+    <t>java</t>
+  </si>
+  <si>
+    <t>Juan Perez</t>
+  </si>
+  <si>
+    <t>Carlos Muñoz</t>
   </si>
   <si>
     <t>SF: AA</t>
@@ -53,19 +53,10 @@
     <t>Python</t>
   </si>
   <si>
-    <t>José</t>
-  </si>
-  <si>
-    <t>María</t>
-  </si>
-  <si>
-    <t>SF: RI</t>
-  </si>
-  <si>
-    <t>Inglés</t>
-  </si>
-  <si>
-    <t>Profe de inglés</t>
+    <t>Jorge mundaca</t>
+  </si>
+  <si>
+    <t>Claudia nog</t>
   </si>
 </sst>
 </file>
@@ -116,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -125,9 +116,9 @@
     <col min="1" max="1" width="7.3515625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="7.37890625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="17.70703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.26953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.5546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="8.26171875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.27734375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="12.73828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="7.21875" customWidth="true" bestFit="true"/>
   </cols>
@@ -172,13 +163,13 @@
         <v>9</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>850000.0</v>
+        <v>1450000.0</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>10</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>11</v>
@@ -186,54 +177,28 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>1111.0</v>
+        <v>2222.0</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>12</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>60.0</v>
+        <v>70.0</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>13</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>980000.0</v>
+        <v>1450000.0</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>14</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>4.666666666666667</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
-        <v>3333.0</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>30.0</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>1582000.0</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>